<commit_message>
Update Exercises and Finish Printing
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9b5b96fb5cf22e04/Projects/Workout-Maker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{DBE8D4D3-7327-4F70-9FB4-9605C8611BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D4A4CEA-37D1-4A38-835D-C18E23C70BF3}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{DBE8D4D3-7327-4F70-9FB4-9605C8611BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E51BD76-3276-4FB4-9B07-A2FB14D98D2B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{03F41662-72BD-43F4-9730-B37408DE9552}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{03F41662-72BD-43F4-9730-B37408DE9552}"/>
   </bookViews>
   <sheets>
     <sheet name="armExercises" sheetId="1" r:id="rId1"/>
@@ -38,66 +38,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
-  <si>
-    <t>exercise1</t>
-  </si>
-  <si>
-    <t>exercise2</t>
-  </si>
-  <si>
-    <t>exercise3</t>
-  </si>
-  <si>
-    <t>exercise4</t>
-  </si>
-  <si>
-    <t>exercise5</t>
-  </si>
-  <si>
-    <t>exercise6</t>
-  </si>
-  <si>
-    <t>exercise7</t>
-  </si>
-  <si>
-    <t>exercise8</t>
-  </si>
-  <si>
-    <t>exercise9</t>
-  </si>
-  <si>
-    <t>exercise10</t>
-  </si>
-  <si>
-    <t>exercise11</t>
-  </si>
-  <si>
-    <t>exercise12</t>
-  </si>
-  <si>
-    <t>exercise13</t>
-  </si>
-  <si>
-    <t>exercise14</t>
-  </si>
-  <si>
-    <t>exercise15</t>
-  </si>
-  <si>
-    <t>exercise16</t>
-  </si>
-  <si>
-    <t>exercise17</t>
-  </si>
-  <si>
-    <t>exercise18</t>
-  </si>
-  <si>
-    <t>exercise19</t>
-  </si>
-  <si>
-    <t>exercise20</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>Burpees</t>
+  </si>
+  <si>
+    <t>Front Squat</t>
+  </si>
+  <si>
+    <t>Hip Bridge</t>
+  </si>
+  <si>
+    <t>Calf Raise</t>
+  </si>
+  <si>
+    <t>Split Squat</t>
+  </si>
+  <si>
+    <t>Crunches</t>
+  </si>
+  <si>
+    <t>Bicycle Crunches (Total)</t>
+  </si>
+  <si>
+    <t>Lunges (Each)</t>
+  </si>
+  <si>
+    <t>Single Calf Raise (Each)</t>
+  </si>
+  <si>
+    <t>Heel Touch (Total)</t>
+  </si>
+  <si>
+    <t>Russian Twists (Total)</t>
+  </si>
+  <si>
+    <t>Leg Raise</t>
+  </si>
+  <si>
+    <t>Toe Touch</t>
+  </si>
+  <si>
+    <t>Forward Circles</t>
+  </si>
+  <si>
+    <t>Squat Pulses</t>
+  </si>
+  <si>
+    <t>Lunge Pulses</t>
+  </si>
+  <si>
+    <t>Side Crunch (Each)</t>
+  </si>
+  <si>
+    <t>Backward Circles</t>
+  </si>
+  <si>
+    <t>Prayer Pulse</t>
+  </si>
+  <si>
+    <t>Knee Push Ups</t>
+  </si>
+  <si>
+    <t>Flutter Kicks (Total)</t>
+  </si>
+  <si>
+    <t>Criss-Cross (Total)</t>
+  </si>
+  <si>
+    <t>Reverse Crunches</t>
+  </si>
+  <si>
+    <t>Elbow-to-Knee (Each)</t>
+  </si>
+  <si>
+    <t>Single Leg Bridge (Each)</t>
+  </si>
+  <si>
+    <t>Lateral Lunge</t>
+  </si>
+  <si>
+    <t>Wall Sit</t>
+  </si>
+  <si>
+    <t>Side to Side (Total)</t>
+  </si>
+  <si>
+    <t>L-Folds</t>
+  </si>
+  <si>
+    <t>Crossover Lunge (Each)</t>
+  </si>
+  <si>
+    <t>Arm Flip (Total)</t>
+  </si>
+  <si>
+    <t>C Rotations</t>
+  </si>
+  <si>
+    <t>L Chest Press</t>
+  </si>
+  <si>
+    <t>Tricep Dips</t>
   </si>
 </sst>
 </file>
@@ -455,89 +497,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83809423-99D5-4EDC-B3FD-EF48107EBBFD}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C1">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -545,145 +587,35 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
         <v>12</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -694,86 +626,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508DA582-9F26-4797-A95E-926352309326}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -781,145 +716,46 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
         <v>12</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -929,23 +765,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D2C7A7-BBED-42C2-BBF4-2D0DFA047E76}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="A14:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -953,208 +792,131 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
       <c r="C7">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
         <v>12</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>